<commit_message>
Teleop and Finish ready
</commit_message>
<xml_diff>
--- a/2017 Zou Keepers RI3D Project Management.xlsx
+++ b/2017 Zou Keepers RI3D Project Management.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aeblab\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Robot Main.vi" sheetId="1" r:id="rId1"/>
@@ -20,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="163">
   <si>
     <t>Joystick_R</t>
   </si>
@@ -124,9 +119,6 @@
     <t>Get Vision Result</t>
   </si>
   <si>
-    <t>Implement_1</t>
-  </si>
-  <si>
     <t>Distance</t>
   </si>
   <si>
@@ -154,9 +146,6 @@
     <t>Owner(s)</t>
   </si>
   <si>
-    <t>Solenoid_1</t>
-  </si>
-  <si>
     <t>Horiz</t>
   </si>
   <si>
@@ -211,12 +200,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Flywheel_L</t>
-  </si>
-  <si>
-    <t>Flywheel_R</t>
-  </si>
-  <si>
     <t>Drive_Forward</t>
   </si>
   <si>
@@ -232,12 +215,6 @@
     <t>AI_1</t>
   </si>
   <si>
-    <t>Pusher</t>
-  </si>
-  <si>
-    <t>Actuator</t>
-  </si>
-  <si>
     <t>(RBG_HSL_Lookup)</t>
   </si>
   <si>
@@ -280,9 +257,6 @@
     <t>Twist</t>
   </si>
   <si>
-    <t>Left=Talon SRX(inverted), Right=Talon SRX</t>
-  </si>
-  <si>
     <t>[dbl], [bool]</t>
   </si>
   <si>
@@ -328,9 +302,6 @@
     <t>Collect</t>
   </si>
   <si>
-    <t>Talon SRX</t>
-  </si>
-  <si>
     <t>Motor Controller???</t>
   </si>
   <si>
@@ -424,9 +395,6 @@
     <t>Forward, Twist</t>
   </si>
   <si>
-    <t>Range</t>
-  </si>
-  <si>
     <t>Cam_Angle</t>
   </si>
   <si>
@@ -443,13 +411,106 @@
   </si>
   <si>
     <t>Init Outlet_Flap</t>
+  </si>
+  <si>
+    <t>Close Joystick_L</t>
+  </si>
+  <si>
+    <t>Close Joystick_R</t>
+  </si>
+  <si>
+    <t>Close Drive</t>
+  </si>
+  <si>
+    <t>Close Flywheel</t>
+  </si>
+  <si>
+    <t>Close Grabber</t>
+  </si>
+  <si>
+    <t>Close Lifter</t>
+  </si>
+  <si>
+    <t>Close Compressor</t>
+  </si>
+  <si>
+    <t>Close Climb</t>
+  </si>
+  <si>
+    <t>Close Collect</t>
+  </si>
+  <si>
+    <t>Close Cam_Angle</t>
+  </si>
+  <si>
+    <t>Close Inlet_Flap</t>
+  </si>
+  <si>
+    <t>Close Outlet_Flap</t>
+  </si>
+  <si>
+    <t>Close Accel</t>
+  </si>
+  <si>
+    <t>Close Gyro</t>
+  </si>
+  <si>
+    <t>Close Drive_L</t>
+  </si>
+  <si>
+    <t>Close Drive_R</t>
+  </si>
+  <si>
+    <t>Close Fly_RPMs</t>
+  </si>
+  <si>
+    <t>Close Switch_Ball</t>
+  </si>
+  <si>
+    <t>Close Switch_Climbed</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> = 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> = top3 toggle</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> = top4 toggle</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> = bottom7 + bottom8</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> = trigger + Ball? + (Fly_RPMs = ok)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> = thumb</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> = trigger</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> = foreback</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> = case trigger (f = twist, t = vision/pid)</t>
+  </si>
+  <si>
+    <t>Servo</t>
+  </si>
+  <si>
+    <t>Talon SRX (Left = 12, 13; Right = 14, 15)</t>
+  </si>
+  <si>
+    <t>Talon SRX (8)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -556,7 +617,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -611,16 +672,9 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -681,7 +735,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -713,10 +767,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -748,7 +801,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -924,17 +976,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:L85"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:L99"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A51" sqref="A51:XFD52"/>
+      <selection pane="bottomRight" activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="5" width="4.7109375" style="12" customWidth="1"/>
     <col min="6" max="7" width="15.7109375" style="12" customWidth="1"/>
@@ -946,17 +998,17 @@
     <col min="13" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
+    <row r="2" spans="1:12" s="1" customFormat="1">
+      <c r="A2" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
       <c r="G2" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>15</v>
@@ -965,85 +1017,85 @@
         <v>16</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K2" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:12" s="4" customFormat="1">
       <c r="A3" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I3" s="16"/>
       <c r="J3" s="17"/>
     </row>
-    <row r="4" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" s="5" customFormat="1">
       <c r="B4" s="5" t="s">
         <v>19</v>
       </c>
       <c r="G4" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="H4" s="5" t="s">
-        <v>87</v>
-      </c>
       <c r="I4" s="6" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="J4" s="7"/>
-      <c r="K4" s="29" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K4" s="26" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="5" customFormat="1">
       <c r="B5" s="5" t="s">
         <v>18</v>
       </c>
       <c r="G5" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="I5" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="H5" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>88</v>
-      </c>
       <c r="J5" s="7"/>
-      <c r="K5" s="29" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K5" s="26" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="5" customFormat="1">
       <c r="B6" s="5" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="H6" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="J6" s="7"/>
+      <c r="K6" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="5" customFormat="1">
+      <c r="B7" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="I6" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="J6" s="7"/>
-      <c r="K6" s="31" t="s">
-        <v>114</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
-        <v>96</v>
-      </c>
       <c r="G7" s="5" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>13</v>
@@ -1052,19 +1104,19 @@
         <v>1</v>
       </c>
       <c r="J7" s="7"/>
-      <c r="K7" s="31" t="s">
-        <v>114</v>
+      <c r="K7" s="27" t="s">
+        <v>106</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="5" customFormat="1">
       <c r="B8" s="5" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>2</v>
@@ -1073,16 +1125,16 @@
         <v>1</v>
       </c>
       <c r="J8" s="7"/>
-      <c r="K8" s="31" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K8" s="27" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="5" customFormat="1">
       <c r="B9" s="5" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>2</v>
@@ -1091,11 +1143,11 @@
         <v>1</v>
       </c>
       <c r="J9" s="7"/>
-      <c r="K9" s="31" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K9" s="27" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="5" customFormat="1">
       <c r="B10" s="5" t="s">
         <v>32</v>
       </c>
@@ -1109,16 +1161,16 @@
         <v>1</v>
       </c>
       <c r="J10" s="7"/>
-      <c r="K10" s="31" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K10" s="27" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="5" customFormat="1">
       <c r="B11" s="5" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>13</v>
@@ -1128,18 +1180,18 @@
       </c>
       <c r="J11" s="7"/>
       <c r="K11" s="22" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="5" customFormat="1">
       <c r="B12" s="5" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>13</v>
@@ -1149,18 +1201,18 @@
       </c>
       <c r="J12" s="7"/>
       <c r="K12" s="22" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="L12" s="5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" s="5" customFormat="1">
       <c r="B13" s="5" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>13</v>
@@ -1170,15 +1222,18 @@
       </c>
       <c r="J13" s="7"/>
       <c r="K13" s="22" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="5" customFormat="1">
       <c r="B14" s="5" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>13</v>
@@ -1188,15 +1243,18 @@
       </c>
       <c r="J14" s="7"/>
       <c r="K14" s="22" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" s="5" customFormat="1">
       <c r="B15" s="5" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>13</v>
@@ -1206,33 +1264,36 @@
       </c>
       <c r="J15" s="7"/>
       <c r="K15" s="22" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="L15" s="5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" s="5" customFormat="1">
       <c r="B16" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="H16" s="5" t="s">
         <v>124</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>132</v>
       </c>
       <c r="I16" s="6">
         <v>3</v>
       </c>
       <c r="J16" s="7"/>
       <c r="K16" s="20" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" s="5" customFormat="1">
       <c r="B17" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>13</v>
@@ -1242,78 +1303,78 @@
       </c>
       <c r="J17" s="7"/>
       <c r="K17" s="20" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" s="5" customFormat="1">
       <c r="B18" s="5" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I18" s="6">
         <v>1</v>
       </c>
       <c r="J18" s="7"/>
       <c r="K18" s="21" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="L18" s="5" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" s="5" customFormat="1">
       <c r="B19" s="5" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I19" s="6">
         <v>1</v>
       </c>
       <c r="J19" s="7"/>
       <c r="K19" s="21" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="L19" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" s="5" customFormat="1">
+      <c r="B20" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G20" s="5" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>130</v>
-      </c>
       <c r="H20" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I20" s="6">
         <v>1</v>
       </c>
       <c r="J20" s="7"/>
       <c r="K20" s="21" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="L20" s="5" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" s="5" customFormat="1">
       <c r="B21" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>2</v>
@@ -1323,15 +1384,15 @@
       </c>
       <c r="J21" s="7"/>
       <c r="K21" s="21" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" s="5" customFormat="1">
       <c r="B22" s="5" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="H22" s="5" t="s">
         <v>2</v>
@@ -1341,95 +1402,95 @@
       </c>
       <c r="J22" s="7"/>
       <c r="K22" s="21" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" s="8" customFormat="1">
       <c r="A23" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I23" s="18"/>
       <c r="J23" s="19"/>
     </row>
-    <row r="24" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" s="23" customFormat="1">
       <c r="B24" s="23" t="s">
         <v>20</v>
       </c>
       <c r="I24" s="24"/>
       <c r="J24" s="25"/>
     </row>
-    <row r="25" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" s="23" customFormat="1">
       <c r="B25" s="23" t="s">
         <v>21</v>
       </c>
       <c r="I25" s="24"/>
       <c r="J25" s="25"/>
     </row>
-    <row r="26" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" s="4" customFormat="1">
       <c r="A26" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I26" s="16"/>
       <c r="J26" s="17"/>
     </row>
-    <row r="27" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" s="5" customFormat="1">
       <c r="B27" s="5" t="s">
         <v>17</v>
       </c>
       <c r="I27" s="6"/>
       <c r="J27" s="7"/>
     </row>
-    <row r="28" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" s="5" customFormat="1">
       <c r="C28" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G28" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="H28" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="H28" s="5" t="s">
-        <v>87</v>
-      </c>
       <c r="I28" s="6" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="J28" s="7"/>
     </row>
-    <row r="29" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" s="5" customFormat="1">
       <c r="C29" s="5" t="s">
         <v>0</v>
       </c>
       <c r="G29" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="I29" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="H29" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="I29" s="6" t="s">
-        <v>88</v>
-      </c>
       <c r="J29" s="7"/>
     </row>
-    <row r="30" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" s="5" customFormat="1">
       <c r="C30" s="5" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="I30" s="6">
         <v>3</v>
       </c>
       <c r="J30" s="7"/>
     </row>
-    <row r="31" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" s="5" customFormat="1">
       <c r="C31" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H31" s="5" t="s">
         <v>13</v>
@@ -1439,63 +1500,63 @@
       </c>
       <c r="J31" s="7"/>
     </row>
-    <row r="32" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" s="5" customFormat="1">
       <c r="C32" s="5" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I32" s="6">
         <v>1</v>
       </c>
       <c r="J32" s="7"/>
       <c r="L32" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="33" spans="2:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" s="5" customFormat="1">
       <c r="C33" s="5" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I33" s="6">
         <v>1</v>
       </c>
       <c r="J33" s="7"/>
       <c r="L33" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="34" spans="2:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" s="5" customFormat="1">
       <c r="C34" s="5" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I34" s="6">
         <v>1</v>
       </c>
       <c r="J34" s="7"/>
     </row>
-    <row r="35" spans="2:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:12" s="5" customFormat="1">
       <c r="C35" s="5" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="H35" s="5" t="s">
         <v>2</v>
@@ -1505,12 +1566,12 @@
       </c>
       <c r="J35" s="7"/>
     </row>
-    <row r="36" spans="2:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:12" s="5" customFormat="1">
       <c r="C36" s="5" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="H36" s="5" t="s">
         <v>2</v>
@@ -1520,7 +1581,7 @@
       </c>
       <c r="J36" s="7"/>
     </row>
-    <row r="37" spans="2:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:12" s="5" customFormat="1">
       <c r="C37" s="5" t="s">
         <v>33</v>
       </c>
@@ -1528,86 +1589,98 @@
         <v>3</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I37" s="6">
         <v>1</v>
       </c>
       <c r="J37" s="7"/>
     </row>
-    <row r="38" spans="2:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:12" s="5" customFormat="1">
       <c r="B38" s="5" t="s">
         <v>22</v>
       </c>
       <c r="I38" s="6"/>
       <c r="J38" s="7"/>
     </row>
-    <row r="39" spans="2:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:12" s="5" customFormat="1">
       <c r="C39" s="5" t="s">
-        <v>65</v>
+        <v>110</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
       <c r="H39" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="I39" s="6">
+        <v>1</v>
+      </c>
+      <c r="J39" s="7"/>
+      <c r="L39" s="5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" s="5" customFormat="1">
+      <c r="C40" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="I40" s="6">
+        <v>1</v>
+      </c>
+      <c r="J40" s="7"/>
+      <c r="L40" s="5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12" s="5" customFormat="1">
+      <c r="C41" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="H41" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="I39" s="6">
-        <v>1</v>
-      </c>
-      <c r="J39" s="7"/>
-    </row>
-    <row r="40" spans="2:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C40" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="G40" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="H40" s="5" t="s">
+      <c r="I41" s="6">
+        <v>1</v>
+      </c>
+      <c r="J41" s="7"/>
+      <c r="L41" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="42" spans="2:12" s="5" customFormat="1">
+      <c r="C42" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="H42" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="I40" s="6">
-        <v>1</v>
-      </c>
-      <c r="J40" s="7"/>
-    </row>
-    <row r="41" spans="2:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C41" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="G41" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="H41" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="I41" s="6">
-        <v>1</v>
-      </c>
-      <c r="J41" s="7"/>
-    </row>
-    <row r="42" spans="2:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C42" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="G42" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="H42" s="5" t="s">
-        <v>2</v>
-      </c>
       <c r="I42" s="6">
         <v>1</v>
       </c>
       <c r="J42" s="7"/>
-    </row>
-    <row r="43" spans="2:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L42" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="43" spans="2:12" s="5" customFormat="1">
       <c r="C43" s="5" t="s">
-        <v>99</v>
+        <v>126</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>99</v>
+        <v>126</v>
       </c>
       <c r="H43" s="5" t="s">
         <v>13</v>
@@ -1617,12 +1690,12 @@
       </c>
       <c r="J43" s="7"/>
     </row>
-    <row r="44" spans="2:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:12" s="5" customFormat="1">
       <c r="C44" s="5" t="s">
-        <v>101</v>
+        <v>128</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>101</v>
+        <v>128</v>
       </c>
       <c r="H44" s="5" t="s">
         <v>13</v>
@@ -1631,13 +1704,16 @@
         <v>1</v>
       </c>
       <c r="J44" s="7"/>
-    </row>
-    <row r="45" spans="2:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L44" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12" s="5" customFormat="1">
       <c r="C45" s="5" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="H45" s="5" t="s">
         <v>13</v>
@@ -1646,13 +1722,16 @@
         <v>1</v>
       </c>
       <c r="J45" s="7"/>
-    </row>
-    <row r="46" spans="2:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L45" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="46" spans="2:12" s="5" customFormat="1">
       <c r="C46" s="5" t="s">
-        <v>137</v>
+        <v>91</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>137</v>
+        <v>76</v>
       </c>
       <c r="H46" s="5" t="s">
         <v>13</v>
@@ -1661,13 +1740,16 @@
         <v>1</v>
       </c>
       <c r="J46" s="7"/>
-    </row>
-    <row r="47" spans="2:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L46" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12" s="5" customFormat="1">
       <c r="C47" s="5" t="s">
-        <v>138</v>
+        <v>61</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>138</v>
+        <v>78</v>
       </c>
       <c r="H47" s="5" t="s">
         <v>13</v>
@@ -1676,13 +1758,16 @@
         <v>1</v>
       </c>
       <c r="J47" s="7"/>
-    </row>
-    <row r="48" spans="2:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L47" s="5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="48" spans="2:12" s="5" customFormat="1">
       <c r="C48" s="5" t="s">
-        <v>134</v>
+        <v>62</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>134</v>
+        <v>79</v>
       </c>
       <c r="H48" s="5" t="s">
         <v>13</v>
@@ -1691,305 +1776,355 @@
         <v>1</v>
       </c>
       <c r="J48" s="7"/>
-    </row>
-    <row r="49" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C49" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="G49" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="H49" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="I49" s="6">
-        <v>1</v>
-      </c>
+      <c r="L48" s="5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" s="5" customFormat="1">
+      <c r="B49" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I49" s="6"/>
       <c r="J49" s="7"/>
     </row>
-    <row r="50" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" s="5" customFormat="1">
+      <c r="C50" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>78</v>
+      </c>
       <c r="I50" s="6"/>
       <c r="J50" s="7"/>
     </row>
-    <row r="51" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="I51" s="27"/>
-      <c r="J51" s="28"/>
-    </row>
-    <row r="52" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="I52" s="27"/>
-      <c r="J52" s="28"/>
-    </row>
-    <row r="53" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="5" t="s">
-        <v>14</v>
+    <row r="51" spans="1:10" s="5" customFormat="1">
+      <c r="C51" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="I51" s="6"/>
+      <c r="J51" s="7"/>
+    </row>
+    <row r="52" spans="1:10" s="5" customFormat="1">
+      <c r="C52" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="I52" s="6"/>
+      <c r="J52" s="7"/>
+    </row>
+    <row r="53" spans="1:10" s="5" customFormat="1">
+      <c r="C53" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="G53" s="5" t="s">
+        <v>110</v>
       </c>
       <c r="I53" s="6"/>
       <c r="J53" s="7"/>
     </row>
-    <row r="54" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" s="5" customFormat="1">
       <c r="C54" s="5" t="s">
-        <v>65</v>
+        <v>112</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>112</v>
       </c>
       <c r="I54" s="6"/>
       <c r="J54" s="7"/>
     </row>
-    <row r="55" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" s="5" customFormat="1">
       <c r="C55" s="5" t="s">
-        <v>66</v>
+        <v>92</v>
+      </c>
+      <c r="G55" s="5" t="s">
+        <v>92</v>
       </c>
       <c r="I55" s="6"/>
       <c r="J55" s="7"/>
     </row>
-    <row r="56" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" s="5" customFormat="1">
       <c r="C56" s="5" t="s">
-        <v>71</v>
+        <v>94</v>
+      </c>
+      <c r="G56" s="5" t="s">
+        <v>94</v>
       </c>
       <c r="I56" s="6"/>
       <c r="J56" s="7"/>
     </row>
-    <row r="57" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" s="5" customFormat="1">
       <c r="C57" s="5" t="s">
-        <v>63</v>
+        <v>126</v>
+      </c>
+      <c r="G57" s="5" t="s">
+        <v>126</v>
       </c>
       <c r="I57" s="6"/>
       <c r="J57" s="7"/>
     </row>
-    <row r="58" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" s="5" customFormat="1">
       <c r="C58" s="5" t="s">
-        <v>64</v>
+        <v>128</v>
+      </c>
+      <c r="G58" s="5" t="s">
+        <v>128</v>
       </c>
       <c r="I58" s="6"/>
       <c r="J58" s="7"/>
     </row>
-    <row r="59" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" s="5" customFormat="1">
       <c r="C59" s="5" t="s">
-        <v>70</v>
+        <v>129</v>
+      </c>
+      <c r="G59" s="5" t="s">
+        <v>129</v>
       </c>
       <c r="I59" s="6"/>
       <c r="J59" s="7"/>
     </row>
-    <row r="60" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C60" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="I60" s="27"/>
-      <c r="J60" s="28"/>
-    </row>
-    <row r="61" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C61" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="I61" s="27"/>
-      <c r="J61" s="28"/>
-    </row>
-    <row r="62" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="I62" s="18"/>
-      <c r="J62" s="19"/>
-    </row>
-    <row r="63" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" s="8" customFormat="1">
+      <c r="A60" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="I60" s="18"/>
+      <c r="J60" s="19"/>
+    </row>
+    <row r="61" spans="1:10" s="9" customFormat="1">
+      <c r="B61" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I61" s="10"/>
+      <c r="J61" s="11"/>
+    </row>
+    <row r="62" spans="1:10" s="9" customFormat="1">
+      <c r="B62" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I62" s="10"/>
+      <c r="J62" s="11"/>
+    </row>
+    <row r="63" spans="1:10" s="9" customFormat="1">
       <c r="B63" s="9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I63" s="10"/>
       <c r="J63" s="11"/>
     </row>
-    <row r="64" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="I64" s="10"/>
-      <c r="J64" s="11"/>
-    </row>
-    <row r="65" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="I65" s="10"/>
-      <c r="J65" s="11"/>
-    </row>
-    <row r="66" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="I66" s="16"/>
-      <c r="J66" s="17" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" s="4" customFormat="1">
+      <c r="A64" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I64" s="16"/>
+      <c r="J64" s="17" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" s="5" customFormat="1">
+      <c r="B65" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G65" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H65" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I65" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="J65" s="7"/>
+    </row>
+    <row r="66" spans="1:10" s="5" customFormat="1">
+      <c r="B66" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G66" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H66" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I66" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="J66" s="7"/>
+    </row>
+    <row r="67" spans="1:10" s="5" customFormat="1">
       <c r="B67" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H67" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I67" s="6" t="s">
         <v>52</v>
       </c>
       <c r="J67" s="7"/>
     </row>
-    <row r="68" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" s="5" customFormat="1">
       <c r="B68" s="5" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>6</v>
+        <v>67</v>
       </c>
       <c r="H68" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I68" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J68" s="7"/>
     </row>
-    <row r="69" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" s="5" customFormat="1">
       <c r="B69" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H69" s="5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I69" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J69" s="7"/>
     </row>
-    <row r="70" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" s="5" customFormat="1">
       <c r="B70" s="5" t="s">
-        <v>72</v>
+        <v>27</v>
       </c>
       <c r="G70" s="5" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="H70" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I70" s="6" t="s">
-        <v>54</v>
+        <v>11</v>
+      </c>
+      <c r="I70" s="6">
+        <v>120</v>
       </c>
       <c r="J70" s="7"/>
     </row>
-    <row r="71" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" s="5" customFormat="1">
       <c r="B71" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G71" s="5" t="s">
-        <v>9</v>
+        <v>46</v>
       </c>
       <c r="H71" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I71" s="6" t="s">
-        <v>54</v>
+        <v>11</v>
+      </c>
+      <c r="I71" s="6">
+        <v>160</v>
       </c>
       <c r="J71" s="7"/>
     </row>
-    <row r="72" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" s="5" customFormat="1">
       <c r="B72" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G72" s="5" t="s">
         <v>47</v>
       </c>
       <c r="H72" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I72" s="6">
-        <v>120</v>
+        <v>54</v>
+      </c>
+      <c r="I72" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="J72" s="7"/>
     </row>
-    <row r="73" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="5" t="s">
-        <v>28</v>
+    <row r="73" spans="1:10" s="5" customFormat="1">
+      <c r="C73" s="5" t="s">
+        <v>43</v>
       </c>
       <c r="G73" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H73" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I73" s="6">
+        <v>1</v>
+      </c>
+      <c r="J73" s="7"/>
+    </row>
+    <row r="74" spans="1:10" s="5" customFormat="1">
+      <c r="C74" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G74" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H74" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I74" s="6">
+        <v>1</v>
+      </c>
+      <c r="J74" s="7"/>
+    </row>
+    <row r="75" spans="1:10" s="5" customFormat="1">
+      <c r="B75" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G75" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="H73" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I73" s="6">
-        <v>160</v>
-      </c>
-      <c r="J73" s="7"/>
-    </row>
-    <row r="74" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G74" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="H74" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="I74" s="6" t="s">
+      <c r="H75" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="I75" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J74" s="7"/>
-    </row>
-    <row r="75" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C75" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="G75" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="H75" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="I75" s="6">
-        <v>1</v>
-      </c>
       <c r="J75" s="7"/>
     </row>
-    <row r="76" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" s="5" customFormat="1">
       <c r="C76" s="5" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="G76" s="5" t="s">
-        <v>46</v>
+        <v>86</v>
       </c>
       <c r="H76" s="5" t="s">
-        <v>51</v>
+        <v>13</v>
       </c>
       <c r="I76" s="6">
         <v>1</v>
       </c>
       <c r="J76" s="7"/>
     </row>
-    <row r="77" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="5" t="s">
-        <v>30</v>
+    <row r="77" spans="1:10" s="5" customFormat="1">
+      <c r="C77" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="G77" s="5" t="s">
-        <v>50</v>
+        <v>84</v>
       </c>
       <c r="H77" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="I77" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="I77" s="6">
+        <v>1</v>
       </c>
       <c r="J77" s="7"/>
     </row>
-    <row r="78" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" s="5" customFormat="1">
       <c r="C78" s="5" t="s">
-        <v>35</v>
+        <v>85</v>
       </c>
       <c r="G78" s="5" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="H78" s="5" t="s">
         <v>13</v>
@@ -1999,69 +2134,217 @@
       </c>
       <c r="J78" s="7"/>
     </row>
-    <row r="79" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C79" s="5" t="s">
-        <v>91</v>
+    <row r="79" spans="1:10" s="5" customFormat="1">
+      <c r="B79" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="G79" s="5" t="s">
-        <v>91</v>
+        <v>3</v>
       </c>
       <c r="H79" s="5" t="s">
-        <v>13</v>
+        <v>88</v>
       </c>
       <c r="I79" s="6">
         <v>1</v>
       </c>
       <c r="J79" s="7"/>
     </row>
-    <row r="80" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C80" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="G80" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="H80" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="I80" s="6">
-        <v>1</v>
-      </c>
-      <c r="J80" s="7"/>
-    </row>
-    <row r="81" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B81" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G81" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="H81" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="I81" s="6">
-        <v>1</v>
-      </c>
-      <c r="J81" s="7"/>
-    </row>
-    <row r="82" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="I82" s="18"/>
-      <c r="J82" s="19"/>
-    </row>
-    <row r="83" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" s="8" customFormat="1">
+      <c r="A80" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I80" s="18"/>
+      <c r="J80" s="19"/>
+    </row>
+    <row r="81" spans="2:10" s="9" customFormat="1">
+      <c r="B81" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="G81" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="I81" s="10"/>
+      <c r="J81" s="11"/>
+    </row>
+    <row r="82" spans="2:10" s="9" customFormat="1">
+      <c r="B82" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="G82" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="I82" s="10"/>
+      <c r="J82" s="11"/>
+    </row>
+    <row r="83" spans="2:10" s="9" customFormat="1">
+      <c r="B83" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="G83" s="9" t="s">
+        <v>125</v>
+      </c>
       <c r="I83" s="10"/>
       <c r="J83" s="11"/>
     </row>
-    <row r="84" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:10" s="9" customFormat="1">
+      <c r="B84" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="G84" s="9" t="s">
+        <v>91</v>
+      </c>
       <c r="I84" s="10"/>
       <c r="J84" s="11"/>
     </row>
-    <row r="85" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:10" s="9" customFormat="1">
+      <c r="B85" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="G85" s="9" t="s">
+        <v>110</v>
+      </c>
       <c r="I85" s="10"/>
       <c r="J85" s="11"/>
+    </row>
+    <row r="86" spans="2:10" s="9" customFormat="1">
+      <c r="B86" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="G86" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="I86" s="10"/>
+      <c r="J86" s="11"/>
+    </row>
+    <row r="87" spans="2:10" s="9" customFormat="1">
+      <c r="B87" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="G87" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="I87" s="10"/>
+      <c r="J87" s="11"/>
+    </row>
+    <row r="88" spans="2:10" s="9" customFormat="1">
+      <c r="B88" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="G88" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="I88" s="10"/>
+      <c r="J88" s="11"/>
+    </row>
+    <row r="89" spans="2:10" s="9" customFormat="1">
+      <c r="B89" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="G89" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="I89" s="10"/>
+      <c r="J89" s="11"/>
+    </row>
+    <row r="90" spans="2:10" s="9" customFormat="1">
+      <c r="B90" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="G90" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="I90" s="10"/>
+      <c r="J90" s="11"/>
+    </row>
+    <row r="91" spans="2:10" s="9" customFormat="1">
+      <c r="B91" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="G91" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="I91" s="10"/>
+      <c r="J91" s="11"/>
+    </row>
+    <row r="92" spans="2:10" s="9" customFormat="1">
+      <c r="B92" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="G92" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="I92" s="10"/>
+      <c r="J92" s="11"/>
+    </row>
+    <row r="93" spans="2:10" s="9" customFormat="1">
+      <c r="B93" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="G93" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="I93" s="10"/>
+      <c r="J93" s="11"/>
+    </row>
+    <row r="94" spans="2:10" s="9" customFormat="1">
+      <c r="B94" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="G94" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="I94" s="10"/>
+      <c r="J94" s="11"/>
+    </row>
+    <row r="95" spans="2:10" s="9" customFormat="1">
+      <c r="B95" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="G95" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="I95" s="10"/>
+      <c r="J95" s="11"/>
+    </row>
+    <row r="96" spans="2:10" s="9" customFormat="1">
+      <c r="B96" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="G96" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="I96" s="10"/>
+      <c r="J96" s="11"/>
+    </row>
+    <row r="97" spans="2:10" s="9" customFormat="1">
+      <c r="B97" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="G97" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="I97" s="10"/>
+      <c r="J97" s="11"/>
+    </row>
+    <row r="98" spans="2:10" s="9" customFormat="1">
+      <c r="B98" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="G98" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="I98" s="10"/>
+      <c r="J98" s="11"/>
+    </row>
+    <row r="99" spans="2:10" s="9" customFormat="1">
+      <c r="B99" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="G99" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="I99" s="10"/>
+      <c r="J99" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2073,14 +2356,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>